<commit_message>
Added quiz game creator
</commit_message>
<xml_diff>
--- a/srv/backendv2/birds_data.xlsx
+++ b/srv/backendv2/birds_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PM34NO\PycharmProjects\bird-site\srv\backendv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A124F4AD-DAE5-414E-9B03-3C7B6256EFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9009A138-A8A5-4357-BA89-581D65FEE4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
   <si>
     <t>suborder</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>small</t>
-  </si>
-  <si>
-    <t>medium</t>
   </si>
   <si>
     <t>TEMP</t>
@@ -1138,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148F78D1-3F80-41D4-B513-75EF1C62F7BB}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1208,7 +1205,7 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>72</v>
@@ -1256,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D783D88-BC5B-4F2D-A74B-0A62FDF1BAB4}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1323,7 +1320,7 @@
         <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>